<commit_message>
[Jallal] more code clean up
</commit_message>
<xml_diff>
--- a/ListOfAddressAndCarrierRoute.xlsx
+++ b/ListOfAddressAndCarrierRoute.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>Cleansed Address</t>
   </si>
@@ -48,6 +48,27 @@
   </si>
   <si>
     <t>3272 ALPINE DR, ANN ARBOR, MI 48108-1766</t>
+  </si>
+  <si>
+    <t>2175 E JOY RD, ANN ARBOR, MI 48105-9230</t>
+  </si>
+  <si>
+    <t>48105-R007</t>
+  </si>
+  <si>
+    <t>2876 BUTTERNUT ST, ANN ARBOR, MI 48108-1851</t>
+  </si>
+  <si>
+    <t>48108-C024</t>
+  </si>
+  <si>
+    <t>1793 ADDINGTON LN, ANN ARBOR, MI 48108-8956</t>
+  </si>
+  <si>
+    <t>1698 POND SHORE DR, ANN ARBOR, MI 48108-9566</t>
+  </si>
+  <si>
+    <t>48108-R005</t>
   </si>
 </sst>
 </file>
@@ -92,7 +113,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -164,58 +185,34 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>